<commit_message>
updated projectTimeline.xlsx . added text document projTimeline
</commit_message>
<xml_diff>
--- a/projectTimetable.xlsx
+++ b/projectTimetable.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">Task 1: Finalize needed tables and attributes (Ary Hernandez, Andrew Samuel, Jacquelyn Johnson)</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 2: Write code using SQL for the database (Andrew Samuel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 3: Implement database within an application (Jacquelyn Johnson) </t>
+    <t xml:space="preserve">Task 2: Write code using SQL for the database (Andrew Samuel (lead), Ary Hernandez, Jacquelyn Johnson)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 3: Implement database within an application (Jacquelyn Johnson (lead), Andrew Samuel, Ary Hernandez) </t>
   </si>
   <si>
     <t xml:space="preserve">March</t>
@@ -58,6 +58,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,12 +80,14 @@
       <color rgb="FF168253"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF168253"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -93,6 +96,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -289,10 +293,10 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.51"/>
   </cols>
@@ -339,7 +343,7 @@
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>

</xml_diff>

<commit_message>
updated projectTimeline.xlsx and text document projTimeline
</commit_message>
<xml_diff>
--- a/projectTimetable.xlsx
+++ b/projectTimetable.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Task 1: Finalize needed tables and attributes (Ary Hernandez, Andrew Samuel, Jacquelyn Johnson)</t>
   </si>
   <si>
-    <t xml:space="preserve">Task 2: Write code using SQL for the database (Andrew Samuel (lead), Ary Hernandez, Jacquelyn Johnson)</t>
+    <t xml:space="preserve">Task 2: Write code using MySQL for the database (Andrew Samuel (lead), Ary Hernandez, Jacquelyn Johnson)</t>
   </si>
   <si>
     <t xml:space="preserve">Task 3: Implement database within an application (Jacquelyn Johnson (lead), Andrew Samuel, Ary Hernandez) </t>
@@ -293,10 +293,10 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.51"/>
   </cols>

</xml_diff>

<commit_message>
added phase2Report. needs further revision
</commit_message>
<xml_diff>
--- a/projectTimetable.xlsx
+++ b/projectTimetable.xlsx
@@ -293,10 +293,10 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.51"/>
   </cols>

</xml_diff>